<commit_message>
Creación de gráficos en Excel
</commit_message>
<xml_diff>
--- a/Excel/Práctica/6. Gráficos en Excel/Creación de gráficos y mini-gráficos en Excel.xlsx
+++ b/Excel/Práctica/6. Gráficos en Excel/Creación de gráficos y mini-gráficos en Excel.xlsx
@@ -790,7 +790,13 @@
     <xf numFmtId="44" fontId="5" fillId="4" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="5" fillId="9" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="9" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -799,17 +805,11 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -860,7 +860,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1174,11 +1173,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2072253840"/>
-        <c:axId val="-2072349616"/>
+        <c:axId val="-2102889920"/>
+        <c:axId val="-2102886192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2072253840"/>
+        <c:axId val="-2102889920"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1221,7 +1220,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2072349616"/>
+        <c:crossAx val="-2102886192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1229,7 +1228,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2072349616"/>
+        <c:axId val="-2102886192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1280,7 +1279,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2072253840"/>
+        <c:crossAx val="-2102889920"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1294,7 +1293,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1507,11 +1505,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2099750704"/>
-        <c:axId val="-2099756928"/>
+        <c:axId val="-2103866208"/>
+        <c:axId val="-2103862544"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2099750704"/>
+        <c:axId val="-2103866208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1554,7 +1552,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2099756928"/>
+        <c:crossAx val="-2103862544"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1562,7 +1560,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2099756928"/>
+        <c:axId val="-2103862544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1613,7 +1611,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2099750704"/>
+        <c:crossAx val="-2103866208"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1808,11 +1806,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="2120241280"/>
-        <c:axId val="2117980816"/>
+        <c:axId val="-2102819632"/>
+        <c:axId val="-2102815968"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="2120241280"/>
+        <c:axId val="-2102819632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1855,7 +1853,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2117980816"/>
+        <c:crossAx val="-2102815968"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1863,7 +1861,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="2117980816"/>
+        <c:axId val="-2102815968"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1914,7 +1912,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2120241280"/>
+        <c:crossAx val="-2102819632"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2403,11 +2401,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-2105820608"/>
-        <c:axId val="-2101721120"/>
+        <c:axId val="-2102086016"/>
+        <c:axId val="-2102082288"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2105820608"/>
+        <c:axId val="-2102086016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2449,7 +2447,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2101721120"/>
+        <c:crossAx val="-2102082288"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2457,7 +2455,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2101721120"/>
+        <c:axId val="-2102082288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2507,7 +2505,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2105820608"/>
+        <c:crossAx val="-2102086016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2646,9 +2644,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2665,15 +2662,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>'Reporte Mensual Primer Año'!$B$3:$G$3</c:f>
@@ -2727,6 +2726,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2736,13 +2736,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-2070854576"/>
-        <c:axId val="-2070851648"/>
-      </c:barChart>
+        <c:smooth val="0"/>
+        <c:axId val="-2131730800"/>
+        <c:axId val="-2131734480"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="-2070854576"/>
+        <c:axId val="-2131730800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2785,7 +2784,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2070851648"/>
+        <c:crossAx val="-2131734480"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2793,7 +2792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2070851648"/>
+        <c:axId val="-2131734480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2844,7 +2843,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2070854576"/>
+        <c:crossAx val="-2131730800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2941,9 +2940,8 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
@@ -2960,15 +2958,17 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
           <c:cat>
             <c:strRef>
               <c:f>'Reporte Mensual Primer Año'!$B$3:$G$3</c:f>
@@ -3022,6 +3022,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="0"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3031,13 +3032,12 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="-2085511936"/>
-        <c:axId val="-2085483968"/>
-      </c:barChart>
+        <c:smooth val="0"/>
+        <c:axId val="-2101128656"/>
+        <c:axId val="-2101124992"/>
+      </c:lineChart>
       <c:catAx>
-        <c:axId val="-2085511936"/>
+        <c:axId val="-2101128656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3080,7 +3080,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2085483968"/>
+        <c:crossAx val="-2101124992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3088,7 +3088,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2085483968"/>
+        <c:axId val="-2101124992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3139,7 +3139,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2085511936"/>
+        <c:crossAx val="-2101128656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6482,7 +6482,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47A410DA-A33D-4A07-9A21-62747AA3CF8F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47A410DA-A33D-4A07-9A21-62747AA3CF8F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6515,7 +6515,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CD43E180-1B68-432D-AA0E-AA69D4E43879}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD43E180-1B68-432D-AA0E-AA69D4E43879}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6548,7 +6548,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8A34D487-923E-4EDE-81B7-48300A01A3EF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A34D487-923E-4EDE-81B7-48300A01A3EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6979,15 +6979,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="24" t="s">
@@ -7027,7 +7027,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -7036,7 +7036,7 @@
       <c r="C6" s="6">
         <v>1000</v>
       </c>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="30" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="20" t="s">
@@ -7047,14 +7047,14 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="31"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="7">
         <v>250</v>
       </c>
-      <c r="E7" s="31"/>
+      <c r="E7" s="30"/>
       <c r="F7" s="21" t="s">
         <v>13</v>
       </c>
@@ -7063,7 +7063,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="31" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="22" t="s">
@@ -7072,7 +7072,7 @@
       <c r="C8" s="8">
         <v>1000</v>
       </c>
-      <c r="E8" s="31"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="20" t="s">
         <v>14</v>
       </c>
@@ -7081,14 +7081,14 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="30"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="7">
         <v>500</v>
       </c>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="33" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="21" t="s">
@@ -7099,7 +7099,7 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="31" t="s">
+      <c r="A10" s="30" t="s">
         <v>34</v>
       </c>
       <c r="B10" s="22" t="s">
@@ -7108,7 +7108,7 @@
       <c r="C10" s="8">
         <v>1000</v>
       </c>
-      <c r="E10" s="28"/>
+      <c r="E10" s="33"/>
       <c r="F10" s="20" t="s">
         <v>13</v>
       </c>
@@ -7117,14 +7117,14 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="31"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="7">
         <v>500</v>
       </c>
-      <c r="E11" s="31" t="s">
+      <c r="E11" s="30" t="s">
         <v>34</v>
       </c>
       <c r="F11" s="20" t="s">
@@ -7135,7 +7135,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="31" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="22" t="s">
@@ -7144,7 +7144,7 @@
       <c r="C12" s="8">
         <v>1000</v>
       </c>
-      <c r="E12" s="31"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="21" t="s">
         <v>13</v>
       </c>
@@ -7153,14 +7153,14 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="30"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="7">
         <v>500</v>
       </c>
-      <c r="E13" s="31"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="20" t="s">
         <v>14</v>
       </c>
@@ -7169,7 +7169,7 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="31" t="s">
+      <c r="A14" s="30" t="s">
         <v>27</v>
       </c>
       <c r="B14" s="22" t="s">
@@ -7178,7 +7178,7 @@
       <c r="C14" s="8">
         <v>1000</v>
       </c>
-      <c r="E14" s="28" t="s">
+      <c r="E14" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F14" s="21" t="s">
@@ -7189,14 +7189,14 @@
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="31"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="7">
         <v>700</v>
       </c>
-      <c r="E15" s="28"/>
+      <c r="E15" s="33"/>
       <c r="F15" s="20" t="s">
         <v>13</v>
       </c>
@@ -7205,7 +7205,7 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="31" t="s">
         <v>35</v>
       </c>
       <c r="B16" s="22" t="s">
@@ -7214,7 +7214,7 @@
       <c r="C16" s="8">
         <v>1000</v>
       </c>
-      <c r="E16" s="31" t="s">
+      <c r="E16" s="30" t="s">
         <v>27</v>
       </c>
       <c r="F16" s="21" t="s">
@@ -7225,14 +7225,14 @@
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="30"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="7">
         <v>700</v>
       </c>
-      <c r="E17" s="31"/>
+      <c r="E17" s="30"/>
       <c r="F17" s="20" t="s">
         <v>13</v>
       </c>
@@ -7241,7 +7241,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E18" s="28" t="s">
+      <c r="E18" s="33" t="s">
         <v>35</v>
       </c>
       <c r="F18" s="21" t="s">
@@ -7252,7 +7252,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E19" s="28"/>
+      <c r="E19" s="33"/>
       <c r="F19" s="20" t="s">
         <v>13</v>
       </c>
@@ -7262,12 +7262,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A10:A11"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
@@ -7275,6 +7269,12 @@
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -7286,22 +7286,22 @@
   <dimension ref="A1:R27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -7334,17 +7334,17 @@
       <c r="H3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="J3" s="33" t="s">
+      <c r="J3" s="34" t="s">
         <v>39</v>
       </c>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
-      <c r="M3" s="33"/>
-      <c r="N3" s="33"/>
-      <c r="O3" s="33"/>
-      <c r="P3" s="33"/>
-      <c r="Q3" s="33"/>
-      <c r="R3" s="33"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
+      <c r="M3" s="34"/>
+      <c r="N3" s="34"/>
+      <c r="O3" s="34"/>
+      <c r="P3" s="34"/>
+      <c r="Q3" s="34"/>
+      <c r="R3" s="34"/>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
@@ -7378,15 +7378,15 @@
         <f>SUM(B4:G4)</f>
         <v>9150</v>
       </c>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
-      <c r="M4" s="33"/>
-      <c r="N4" s="33"/>
-      <c r="O4" s="33"/>
-      <c r="P4" s="33"/>
-      <c r="Q4" s="33"/>
-      <c r="R4" s="33"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
+      <c r="M4" s="34"/>
+      <c r="N4" s="34"/>
+      <c r="O4" s="34"/>
+      <c r="P4" s="34"/>
+      <c r="Q4" s="34"/>
+      <c r="R4" s="34"/>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="16" t="s">
@@ -7420,15 +7420,15 @@
         <f>SUM(B5:G5)</f>
         <v>3020</v>
       </c>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
-      <c r="M5" s="33"/>
-      <c r="N5" s="33"/>
-      <c r="O5" s="33"/>
-      <c r="P5" s="33"/>
-      <c r="Q5" s="33"/>
-      <c r="R5" s="33"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="34"/>
+      <c r="N5" s="34"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="34"/>
     </row>
     <row r="6" spans="1:18" ht="20" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="17" t="s">
@@ -7462,26 +7462,26 @@
         <f>SUM(B6:G6)</f>
         <v>6130</v>
       </c>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
-      <c r="M6" s="33"/>
-      <c r="N6" s="33"/>
-      <c r="O6" s="33"/>
-      <c r="P6" s="33"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="33"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
+      <c r="M6" s="34"/>
+      <c r="N6" s="34"/>
+      <c r="O6" s="34"/>
+      <c r="P6" s="34"/>
+      <c r="Q6" s="34"/>
+      <c r="R6" s="34"/>
     </row>
     <row r="7" spans="1:18" ht="20" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="J7" s="33"/>
-      <c r="K7" s="33"/>
-      <c r="L7" s="33"/>
-      <c r="M7" s="33"/>
-      <c r="N7" s="33"/>
-      <c r="O7" s="33"/>
-      <c r="P7" s="33"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="33"/>
+      <c r="J7" s="34"/>
+      <c r="K7" s="34"/>
+      <c r="L7" s="34"/>
+      <c r="M7" s="34"/>
+      <c r="N7" s="34"/>
+      <c r="O7" s="34"/>
+      <c r="P7" s="34"/>
+      <c r="Q7" s="34"/>
+      <c r="R7" s="34"/>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="35" t="s">
@@ -7493,15 +7493,15 @@
       <c r="F8" s="35"/>
       <c r="G8" s="35"/>
       <c r="H8" s="35"/>
-      <c r="J8" s="33"/>
-      <c r="K8" s="33"/>
-      <c r="L8" s="33"/>
-      <c r="M8" s="33"/>
-      <c r="N8" s="33"/>
-      <c r="O8" s="33"/>
-      <c r="P8" s="33"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="33"/>
+      <c r="J8" s="34"/>
+      <c r="K8" s="34"/>
+      <c r="L8" s="34"/>
+      <c r="M8" s="34"/>
+      <c r="N8" s="34"/>
+      <c r="O8" s="34"/>
+      <c r="P8" s="34"/>
+      <c r="Q8" s="34"/>
+      <c r="R8" s="34"/>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B9" s="35"/>
@@ -7511,127 +7511,127 @@
       <c r="F9" s="35"/>
       <c r="G9" s="35"/>
       <c r="H9" s="35"/>
-      <c r="J9" s="33"/>
-      <c r="K9" s="33"/>
-      <c r="L9" s="33"/>
-      <c r="M9" s="33"/>
-      <c r="N9" s="33"/>
-      <c r="O9" s="33"/>
-      <c r="P9" s="33"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="33"/>
+      <c r="J9" s="34"/>
+      <c r="K9" s="34"/>
+      <c r="L9" s="34"/>
+      <c r="M9" s="34"/>
+      <c r="N9" s="34"/>
+      <c r="O9" s="34"/>
+      <c r="P9" s="34"/>
+      <c r="Q9" s="34"/>
+      <c r="R9" s="34"/>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J10" s="34"/>
-      <c r="K10" s="34"/>
-      <c r="L10" s="34"/>
-      <c r="M10" s="34"/>
-      <c r="N10" s="34"/>
-      <c r="O10" s="34"/>
-      <c r="P10" s="34"/>
-      <c r="Q10" s="34"/>
-      <c r="R10" s="34"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="28"/>
+      <c r="L10" s="28"/>
+      <c r="M10" s="28"/>
+      <c r="N10" s="28"/>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28"/>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="28"/>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
-      <c r="L11" s="34"/>
-      <c r="M11" s="34"/>
-      <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
-      <c r="Q11" s="34"/>
-      <c r="R11" s="34"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="28"/>
+      <c r="L11" s="28"/>
+      <c r="M11" s="28"/>
+      <c r="N11" s="28"/>
+      <c r="O11" s="28"/>
+      <c r="P11" s="28"/>
+      <c r="Q11" s="28"/>
+      <c r="R11" s="28"/>
     </row>
     <row r="20" spans="10:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J20" s="33" t="s">
+      <c r="J20" s="34" t="s">
         <v>41</v>
       </c>
-      <c r="K20" s="33"/>
-      <c r="L20" s="33"/>
-      <c r="M20" s="33"/>
-      <c r="N20" s="33"/>
-      <c r="O20" s="33"/>
-      <c r="P20" s="33"/>
-      <c r="Q20" s="33"/>
-      <c r="R20" s="33"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="34"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="34"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="34"/>
     </row>
     <row r="21" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J21" s="33"/>
-      <c r="K21" s="33"/>
-      <c r="L21" s="33"/>
-      <c r="M21" s="33"/>
-      <c r="N21" s="33"/>
-      <c r="O21" s="33"/>
-      <c r="P21" s="33"/>
-      <c r="Q21" s="33"/>
-      <c r="R21" s="33"/>
+      <c r="J21" s="34"/>
+      <c r="K21" s="34"/>
+      <c r="L21" s="34"/>
+      <c r="M21" s="34"/>
+      <c r="N21" s="34"/>
+      <c r="O21" s="34"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="34"/>
     </row>
     <row r="22" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J22" s="33"/>
-      <c r="K22" s="33"/>
-      <c r="L22" s="33"/>
-      <c r="M22" s="33"/>
-      <c r="N22" s="33"/>
-      <c r="O22" s="33"/>
-      <c r="P22" s="33"/>
-      <c r="Q22" s="33"/>
-      <c r="R22" s="33"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
+      <c r="P22" s="34"/>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="34"/>
     </row>
     <row r="23" spans="10:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J23" s="33"/>
-      <c r="K23" s="33"/>
-      <c r="L23" s="33"/>
-      <c r="M23" s="33"/>
-      <c r="N23" s="33"/>
-      <c r="O23" s="33"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="33"/>
-      <c r="R23" s="33"/>
+      <c r="J23" s="34"/>
+      <c r="K23" s="34"/>
+      <c r="L23" s="34"/>
+      <c r="M23" s="34"/>
+      <c r="N23" s="34"/>
+      <c r="O23" s="34"/>
+      <c r="P23" s="34"/>
+      <c r="Q23" s="34"/>
+      <c r="R23" s="34"/>
     </row>
     <row r="24" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
-      <c r="L24" s="34"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="34"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="34"/>
-      <c r="Q24" s="34"/>
-      <c r="R24" s="34"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
+      <c r="P24" s="28"/>
+      <c r="Q24" s="28"/>
+      <c r="R24" s="28"/>
     </row>
     <row r="25" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
-      <c r="L25" s="34"/>
-      <c r="M25" s="34"/>
-      <c r="N25" s="34"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="34"/>
+      <c r="J25" s="28"/>
+      <c r="K25" s="28"/>
+      <c r="L25" s="28"/>
+      <c r="M25" s="28"/>
+      <c r="N25" s="28"/>
+      <c r="O25" s="28"/>
+      <c r="P25" s="28"/>
+      <c r="Q25" s="28"/>
+      <c r="R25" s="28"/>
     </row>
     <row r="26" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J26" s="34"/>
-      <c r="K26" s="34"/>
-      <c r="L26" s="34"/>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
-      <c r="Q26" s="34"/>
-      <c r="R26" s="34"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
+      <c r="P26" s="28"/>
+      <c r="Q26" s="28"/>
+      <c r="R26" s="28"/>
     </row>
     <row r="27" spans="10:18" x14ac:dyDescent="0.25">
-      <c r="J27" s="34"/>
-      <c r="K27" s="34"/>
-      <c r="L27" s="34"/>
-      <c r="M27" s="34"/>
-      <c r="N27" s="34"/>
-      <c r="O27" s="34"/>
-      <c r="P27" s="34"/>
-      <c r="Q27" s="34"/>
-      <c r="R27" s="34"/>
+      <c r="J27" s="28"/>
+      <c r="K27" s="28"/>
+      <c r="L27" s="28"/>
+      <c r="M27" s="28"/>
+      <c r="N27" s="28"/>
+      <c r="O27" s="28"/>
+      <c r="P27" s="28"/>
+      <c r="Q27" s="28"/>
+      <c r="R27" s="28"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -7660,15 +7660,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -7729,7 +7729,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="31" t="s">
+      <c r="A6" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -7739,7 +7739,7 @@
         <v>1200</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="31" t="s">
+      <c r="E6" s="30" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="20" t="s">
@@ -7750,7 +7750,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="31"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="21" t="s">
         <v>18</v>
       </c>
@@ -7758,7 +7758,7 @@
         <v>100</v>
       </c>
       <c r="D7" s="2"/>
-      <c r="E7" s="31"/>
+      <c r="E7" s="30"/>
       <c r="F7" s="21" t="s">
         <v>20</v>
       </c>
@@ -7767,7 +7767,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="28" t="s">
+      <c r="A8" s="33" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="22" t="s">
@@ -7777,7 +7777,7 @@
         <v>1200</v>
       </c>
       <c r="D8" s="2"/>
-      <c r="E8" s="31"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="20" t="s">
         <v>14</v>
       </c>
@@ -7786,7 +7786,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
+      <c r="A9" s="33"/>
       <c r="B9" s="21" t="s">
         <v>22</v>
       </c>
@@ -7794,7 +7794,7 @@
         <v>300</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="28" t="s">
+      <c r="E9" s="33" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="21" t="s">
@@ -7806,7 +7806,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="D10" s="2"/>
-      <c r="E10" s="28"/>
+      <c r="E10" s="33"/>
       <c r="F10" s="20" t="s">
         <v>13</v>
       </c>
@@ -7837,16 +7837,16 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -7991,16 +7991,16 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="29" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="32"/>
-      <c r="F1" s="32"/>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>

</xml_diff>

<commit_message>
Ejercicio de gráficos en Excel
</commit_message>
<xml_diff>
--- a/Excel/Práctica/6. Gráficos en Excel/Creación de gráficos y mini-gráficos en Excel.xlsx
+++ b/Excel/Práctica/6. Gráficos en Excel/Creación de gráficos y mini-gráficos en Excel.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="888" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16540" tabRatio="888" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Primer Año" sheetId="1" r:id="rId1"/>
@@ -153,7 +153,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="45">
   <si>
     <t>Mes</t>
   </si>
@@ -231,9 +231,6 @@
   </si>
   <si>
     <t>Abril</t>
-  </si>
-  <si>
-    <t>etc…</t>
   </si>
   <si>
     <t>Mayo</t>
@@ -554,6 +551,12 @@
       </rPr>
       <t>Diseño de minigráfico.</t>
     </r>
+  </si>
+  <si>
+    <t>Negocios</t>
+  </si>
+  <si>
+    <t>Tenga en cuenta que, generalmente, dentro de los datos seleccionados, para visualizar el mini-gráfico, no se toman valores alfabeticos; no tiene sentido porque en el mini-gráfico no se va a poder visualizar ninguna referencia textual dentro de él (con relación al gráfico en sí), entonces seleccione solo los valores numéricos de su interés, los que desea analizar, a la hora de tomar los datos con los que va a visualizar dicho gráfico.</t>
   </si>
 </sst>
 </file>
@@ -877,7 +880,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -886,11 +892,8 @@
     <xf numFmtId="0" fontId="6" fillId="7" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -944,6 +947,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1257,11 +1261,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2097241568"/>
-        <c:axId val="-2097497200"/>
+        <c:axId val="2094223152"/>
+        <c:axId val="2124512464"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2097241568"/>
+        <c:axId val="2094223152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1304,7 +1308,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097497200"/>
+        <c:crossAx val="2124512464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1312,7 +1316,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2097497200"/>
+        <c:axId val="2124512464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1363,7 +1367,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2097241568"/>
+        <c:crossAx val="2094223152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1377,6 +1381,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1460,6 +1465,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1589,11 +1595,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2069226112"/>
-        <c:axId val="-2069222720"/>
+        <c:axId val="-2109229072"/>
+        <c:axId val="-2109225408"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2069226112"/>
+        <c:axId val="-2109229072"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1636,7 +1642,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2069222720"/>
+        <c:crossAx val="-2109225408"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1644,7 +1650,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2069222720"/>
+        <c:axId val="-2109225408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1695,7 +1701,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2069226112"/>
+        <c:crossAx val="-2109229072"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1761,6 +1767,7 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1890,11 +1897,11 @@
         </c:dLbls>
         <c:gapWidth val="219"/>
         <c:overlap val="-27"/>
-        <c:axId val="-2061242080"/>
-        <c:axId val="-2096982464"/>
+        <c:axId val="-2109184656"/>
+        <c:axId val="-2109180992"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2061242080"/>
+        <c:axId val="-2109184656"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1937,7 +1944,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096982464"/>
+        <c:crossAx val="-2109180992"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1945,7 +1952,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2096982464"/>
+        <c:axId val="-2109180992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1996,7 +2003,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2061242080"/>
+        <c:crossAx val="-2109184656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2485,11 +2492,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="-2061243840"/>
-        <c:axId val="-2061136112"/>
+        <c:axId val="-2110404640"/>
+        <c:axId val="-2110408384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2061243840"/>
+        <c:axId val="-2110404640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2531,7 +2538,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2061136112"/>
+        <c:crossAx val="-2110408384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2539,7 +2546,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2061136112"/>
+        <c:axId val="-2110408384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2589,7 +2596,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2061243840"/>
+        <c:crossAx val="-2110404640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2821,11 +2828,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2130794368"/>
-        <c:axId val="-2130827696"/>
+        <c:axId val="-2112488176"/>
+        <c:axId val="-2112491856"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2130794368"/>
+        <c:axId val="-2112488176"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2868,7 +2875,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2130827696"/>
+        <c:crossAx val="-2112491856"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2876,7 +2883,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2130827696"/>
+        <c:axId val="-2112491856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2927,7 +2934,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2130794368"/>
+        <c:crossAx val="-2112488176"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3117,11 +3124,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-2061099744"/>
-        <c:axId val="-2096709536"/>
+        <c:axId val="-2112523632"/>
+        <c:axId val="-2112527312"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2061099744"/>
+        <c:axId val="-2112523632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3164,7 +3171,7 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2096709536"/>
+        <c:crossAx val="-2112527312"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3172,7 +3179,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2096709536"/>
+        <c:axId val="-2112527312"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3223,7 +3230,602 @@
             <a:endParaRPr lang="es-ES_tradnl"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2061099744"/>
+        <c:crossAx val="-2112523632"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES_tradnl"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-CO"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Reporte Mensual Segundo Año'!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Ingresos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Reporte Mensual Segundo Año'!$B$3:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Enero</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Febrero</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marzo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Reporte Mensual Segundo Año'!$B$4:$G$4</c:f>
+              <c:numCache>
+                <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>1300.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1600.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1400.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1400.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1700.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2070342208"/>
+        <c:axId val="-2070768288"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2070342208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2070768288"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2070768288"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="200.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2070342208"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:majorUnit val="200.0"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="es-ES_tradnl"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="es-CO"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="es-ES_tradnl"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Reporte Mensual Segundo Año'!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Egresos</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Reporte Mensual Segundo Año'!$B$3:$G$3</c:f>
+              <c:strCache>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>Enero</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>Febrero</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>Marzo</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>Abril</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>Mayo</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>Junio</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Reporte Mensual Segundo Año'!$B$5:$G$5</c:f>
+              <c:numCache>
+                <c:formatCode>_-"$"* #,##0.00_-;\-"$"* #,##0.00_-;_-"$"* "-"??_-;_-@_-</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>500.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>400.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>600.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>250.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>700.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="-2097555312"/>
+        <c:axId val="-2066113728"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2097555312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2066113728"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2066113728"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:min val="200.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="es-ES_tradnl"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2097555312"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3512,6 +4114,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -6170,6 +6852,1038 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style8.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6549,7 +8263,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="60" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="125" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -6566,7 +8280,7 @@
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{47A410DA-A33D-4A07-9A21-62747AA3CF8F}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{47A410DA-A33D-4A07-9A21-62747AA3CF8F}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6593,13 +8307,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9302750" cy="6080125"/>
+    <xdr:ext cx="8682182" cy="6292273"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{CD43E180-1B68-432D-AA0E-AA69D4E43879}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CD43E180-1B68-432D-AA0E-AA69D4E43879}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6626,13 +8340,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="9302750" cy="6080125"/>
+    <xdr:ext cx="8676640" cy="6289040"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Gráfico 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{8A34D487-923E-4EDE-81B7-48300A01A3EF}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A34D487-923E-4EDE-81B7-48300A01A3EF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6742,6 +8456,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>901700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Gráfico 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>139700</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>50800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>901700</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Gráfico 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -7063,15 +8842,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B3" s="24" t="s">
@@ -7111,7 +8890,7 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="32" t="s">
+      <c r="A6" s="30" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="20" t="s">
@@ -7120,7 +8899,7 @@
       <c r="C6" s="6">
         <v>1000</v>
       </c>
-      <c r="E6" s="32" t="s">
+      <c r="E6" s="30" t="s">
         <v>8</v>
       </c>
       <c r="F6" s="20" t="s">
@@ -7131,14 +8910,14 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="32"/>
+      <c r="A7" s="30"/>
       <c r="B7" s="21" t="s">
         <v>3</v>
       </c>
       <c r="C7" s="7">
         <v>250</v>
       </c>
-      <c r="E7" s="32"/>
+      <c r="E7" s="30"/>
       <c r="F7" s="21" t="s">
         <v>13</v>
       </c>
@@ -7147,7 +8926,7 @@
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="31" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="22" t="s">
@@ -7156,7 +8935,7 @@
       <c r="C8" s="8">
         <v>1000</v>
       </c>
-      <c r="E8" s="32"/>
+      <c r="E8" s="30"/>
       <c r="F8" s="20" t="s">
         <v>14</v>
       </c>
@@ -7165,14 +8944,14 @@
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="31"/>
+      <c r="A9" s="32"/>
       <c r="B9" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C9" s="7">
         <v>500</v>
       </c>
-      <c r="E9" s="29" t="s">
+      <c r="E9" s="33" t="s">
         <v>9</v>
       </c>
       <c r="F9" s="21" t="s">
@@ -7183,8 +8962,8 @@
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A10" s="32" t="s">
-        <v>34</v>
+      <c r="A10" s="30" t="s">
+        <v>33</v>
       </c>
       <c r="B10" s="22" t="s">
         <v>2</v>
@@ -7192,7 +8971,7 @@
       <c r="C10" s="8">
         <v>1000</v>
       </c>
-      <c r="E10" s="29"/>
+      <c r="E10" s="33"/>
       <c r="F10" s="20" t="s">
         <v>13</v>
       </c>
@@ -7201,15 +8980,15 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A11" s="32"/>
+      <c r="A11" s="30"/>
       <c r="B11" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C11" s="7">
         <v>500</v>
       </c>
-      <c r="E11" s="32" t="s">
-        <v>34</v>
+      <c r="E11" s="30" t="s">
+        <v>33</v>
       </c>
       <c r="F11" s="20" t="s">
         <v>12</v>
@@ -7219,7 +8998,7 @@
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="31" t="s">
         <v>25</v>
       </c>
       <c r="B12" s="22" t="s">
@@ -7228,7 +9007,7 @@
       <c r="C12" s="8">
         <v>1000</v>
       </c>
-      <c r="E12" s="32"/>
+      <c r="E12" s="30"/>
       <c r="F12" s="21" t="s">
         <v>13</v>
       </c>
@@ -7237,14 +9016,14 @@
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A13" s="31"/>
+      <c r="A13" s="32"/>
       <c r="B13" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="7">
         <v>500</v>
       </c>
-      <c r="E13" s="32"/>
+      <c r="E13" s="30"/>
       <c r="F13" s="20" t="s">
         <v>14</v>
       </c>
@@ -7253,8 +9032,8 @@
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A14" s="32" t="s">
-        <v>27</v>
+      <c r="A14" s="30" t="s">
+        <v>26</v>
       </c>
       <c r="B14" s="22" t="s">
         <v>2</v>
@@ -7262,25 +9041,25 @@
       <c r="C14" s="8">
         <v>1000</v>
       </c>
-      <c r="E14" s="29" t="s">
+      <c r="E14" s="33" t="s">
         <v>25</v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="G14" s="13">
         <v>70</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" s="32"/>
+      <c r="A15" s="30"/>
       <c r="B15" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="7">
         <v>700</v>
       </c>
-      <c r="E15" s="29"/>
+      <c r="E15" s="33"/>
       <c r="F15" s="20" t="s">
         <v>13</v>
       </c>
@@ -7289,8 +9068,8 @@
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A16" s="30" t="s">
-        <v>35</v>
+      <c r="A16" s="31" t="s">
+        <v>34</v>
       </c>
       <c r="B16" s="22" t="s">
         <v>2</v>
@@ -7298,25 +9077,25 @@
       <c r="C16" s="8">
         <v>1000</v>
       </c>
-      <c r="E16" s="32" t="s">
-        <v>27</v>
+      <c r="E16" s="30" t="s">
+        <v>26</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="13">
         <v>300</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="31"/>
+      <c r="A17" s="32"/>
       <c r="B17" s="21" t="s">
         <v>5</v>
       </c>
       <c r="C17" s="7">
         <v>700</v>
       </c>
-      <c r="E17" s="32"/>
+      <c r="E17" s="30"/>
       <c r="F17" s="20" t="s">
         <v>13</v>
       </c>
@@ -7325,18 +9104,18 @@
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E18" s="29" t="s">
-        <v>35</v>
+      <c r="E18" s="33" t="s">
+        <v>34</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="G18" s="13">
         <v>800</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="E19" s="29"/>
+      <c r="E19" s="33"/>
       <c r="F19" s="20" t="s">
         <v>13</v>
       </c>
@@ -7346,12 +9125,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="E9:E10"/>
-    <mergeCell ref="A10:A11"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A14:A15"/>
@@ -7359,6 +9132,12 @@
     <mergeCell ref="E11:E13"/>
     <mergeCell ref="E14:E15"/>
     <mergeCell ref="E16:E17"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <legacyDrawing r:id="rId1"/>
@@ -7367,25 +9146,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R27"/>
+  <dimension ref="A1:R32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G28" sqref="G28"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
+      <c r="A1" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -7404,22 +9183,22 @@
         <v>9</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F3" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="H3" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="J3" s="34" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="K3" s="34"/>
       <c r="L3" s="34"/>
@@ -7569,7 +9348,7 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B8" s="35" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="35"/>
       <c r="D8" s="35"/>
@@ -7629,7 +9408,7 @@
     </row>
     <row r="12" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="34" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
@@ -7703,7 +9482,7 @@
     </row>
     <row r="20" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
       <c r="J20" s="34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="K20" s="34"/>
       <c r="L20" s="34"/>
@@ -7755,7 +9534,7 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="B24" s="34" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="34"/>
       <c r="D24" s="34"/>
@@ -7820,14 +9599,596 @@
       <c r="Q27" s="28"/>
       <c r="R27" s="28"/>
     </row>
+    <row r="28" spans="1:18" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="34" t="s">
+        <v>44</v>
+      </c>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="34"/>
+      <c r="F28" s="34"/>
+      <c r="G28" s="34"/>
+      <c r="H28" s="34"/>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B29" s="34"/>
+      <c r="C29" s="34"/>
+      <c r="D29" s="34"/>
+      <c r="E29" s="34"/>
+      <c r="F29" s="34"/>
+      <c r="G29" s="34"/>
+      <c r="H29" s="34"/>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B30" s="34"/>
+      <c r="C30" s="34"/>
+      <c r="D30" s="34"/>
+      <c r="E30" s="34"/>
+      <c r="F30" s="34"/>
+      <c r="G30" s="34"/>
+      <c r="H30" s="34"/>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B31" s="34"/>
+      <c r="C31" s="34"/>
+      <c r="D31" s="34"/>
+      <c r="E31" s="34"/>
+      <c r="F31" s="34"/>
+      <c r="G31" s="34"/>
+      <c r="H31" s="34"/>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="B32" s="34"/>
+      <c r="C32" s="34"/>
+      <c r="D32" s="34"/>
+      <c r="E32" s="34"/>
+      <c r="F32" s="34"/>
+      <c r="G32" s="34"/>
+      <c r="H32" s="34"/>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="B28:H32"/>
     <mergeCell ref="B24:H26"/>
     <mergeCell ref="J20:R23"/>
     <mergeCell ref="B8:H9"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="J3:R9"/>
     <mergeCell ref="B12:H19"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{05C60535-1F16-4fd2-B633-F4F36F0B64E0}">
+      <x14:sparklineGroups xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="gap">
+          <x14:colorSeries theme="4" tint="-0.499984740745262"/>
+          <x14:colorNegative theme="5"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
+          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
+          <x14:colorLast theme="4" tint="0.39997558519241921"/>
+          <x14:colorHigh theme="4"/>
+          <x14:colorLow theme="4"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Reporte Mensual Primer Año'!B4:G4</xm:f>
+              <xm:sqref>B21</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+        <x14:sparklineGroup manualMax="0" manualMin="0" displayEmptyCellsAs="gap">
+          <x14:colorSeries theme="4" tint="-0.499984740745262"/>
+          <x14:colorNegative theme="5"/>
+          <x14:colorAxis rgb="FF000000"/>
+          <x14:colorMarkers theme="4" tint="-0.499984740745262"/>
+          <x14:colorFirst theme="4" tint="0.39997558519241921"/>
+          <x14:colorLast theme="4" tint="0.39997558519241921"/>
+          <x14:colorHigh theme="4"/>
+          <x14:colorLow theme="4"/>
+          <x14:sparklines>
+            <x14:sparkline>
+              <xm:f>'Reporte Mensual Primer Año'!B5:G5</xm:f>
+              <xm:sqref>B22</xm:sqref>
+            </x14:sparkline>
+          </x14:sparklines>
+        </x14:sparklineGroup>
+      </x14:sparklineGroups>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="23" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="24" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="25">
+        <f>SUM(C6:C9)</f>
+        <v>2800</v>
+      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="25">
+        <f>SUM(G6:G10)</f>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
+    </row>
+    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="D5" s="2"/>
+      <c r="E5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="12">
+        <v>1200</v>
+      </c>
+      <c r="D6" s="2"/>
+      <c r="E6" s="30" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="20" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="12">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="30"/>
+      <c r="B7" s="21" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="13">
+        <v>100</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="30"/>
+      <c r="F7" s="21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="23">
+        <v>1200</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="30"/>
+      <c r="F8" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="12">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="33"/>
+      <c r="B9" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="13">
+        <v>300</v>
+      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="33" t="s">
+        <v>9</v>
+      </c>
+      <c r="F9" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="13">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C10" s="23">
+        <v>1400</v>
+      </c>
+      <c r="D10" s="2"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="12">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="33"/>
+      <c r="B11" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="13">
+        <v>200</v>
+      </c>
+      <c r="E11" s="33" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G11" s="13">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="B12" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C12" s="23">
+        <v>1100</v>
+      </c>
+      <c r="E12" s="33"/>
+      <c r="F12" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" s="12">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="33"/>
+      <c r="B13" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="13">
+        <v>300</v>
+      </c>
+      <c r="E13" s="33" t="s">
+        <v>25</v>
+      </c>
+      <c r="F13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="13">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C14" s="23">
+        <v>1200</v>
+      </c>
+      <c r="E14" s="33"/>
+      <c r="F14" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" s="12">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="33"/>
+      <c r="B15" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="13">
+        <v>200</v>
+      </c>
+      <c r="E15" s="33" t="s">
+        <v>26</v>
+      </c>
+      <c r="F15" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G15" s="13">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C16" s="23">
+        <v>1200</v>
+      </c>
+      <c r="E16" s="33"/>
+      <c r="F16" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="12">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" s="33"/>
+      <c r="B17" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="13">
+        <v>500</v>
+      </c>
+      <c r="E17" s="33" t="s">
+        <v>34</v>
+      </c>
+      <c r="F17" s="21" t="s">
+        <v>21</v>
+      </c>
+      <c r="G17" s="13">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E18" s="33"/>
+      <c r="F18" s="20" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="12">
+        <v>300</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="A16:A17"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="E13:E14"/>
+    <mergeCell ref="E15:E16"/>
+    <mergeCell ref="E17:E18"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="E6:E8"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="A10:A11"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.25">
+      <c r="A1" s="29" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+    </row>
+    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
+      <c r="B3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="10">
+        <f>SUM('Segundo Año'!C6:C7)</f>
+        <v>1300</v>
+      </c>
+      <c r="C4" s="10">
+        <f>SUM('Segundo Año'!C8:C9)</f>
+        <v>1500</v>
+      </c>
+      <c r="D4" s="10">
+        <f>SUM('Segundo Año'!C10:C11)</f>
+        <v>1600</v>
+      </c>
+      <c r="E4" s="10">
+        <f>SUM('Segundo Año'!C12:C13)</f>
+        <v>1400</v>
+      </c>
+      <c r="F4" s="10">
+        <f>SUM('Segundo Año'!C14:C15)</f>
+        <v>1400</v>
+      </c>
+      <c r="G4" s="10">
+        <f>SUM('Segundo Año'!C16:D17)</f>
+        <v>1700</v>
+      </c>
+      <c r="H4" s="26">
+        <f>SUM(B4:G4)</f>
+        <v>8900</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="11">
+        <f>SUM('Segundo Año'!G6:G8)</f>
+        <v>600</v>
+      </c>
+      <c r="C5" s="11">
+        <f>SUM('Segundo Año'!G9:G10)</f>
+        <v>500</v>
+      </c>
+      <c r="D5" s="11">
+        <f>SUM('Segundo Año'!G11:G12)</f>
+        <v>400</v>
+      </c>
+      <c r="E5" s="11">
+        <f>SUM('Segundo Año'!G13:G14)</f>
+        <v>600</v>
+      </c>
+      <c r="F5" s="11">
+        <f>SUM('Segundo Año'!G15:G16)</f>
+        <v>250</v>
+      </c>
+      <c r="G5" s="11">
+        <f>SUM('Segundo Año'!G17:G18)</f>
+        <v>700</v>
+      </c>
+      <c r="H5" s="26">
+        <f t="shared" ref="H5:H6" si="0">SUM(B5:G5)</f>
+        <v>3050</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="14">
+        <f>B4-B5</f>
+        <v>700</v>
+      </c>
+      <c r="C6" s="14">
+        <f t="shared" ref="C6:G6" si="1">C4-C5</f>
+        <v>1000</v>
+      </c>
+      <c r="D6" s="14">
+        <f t="shared" si="1"/>
+        <v>1200</v>
+      </c>
+      <c r="E6" s="14">
+        <f t="shared" si="1"/>
+        <v>800</v>
+      </c>
+      <c r="F6" s="14">
+        <f t="shared" si="1"/>
+        <v>1150</v>
+      </c>
+      <c r="G6" s="14">
+        <f>G4-G5</f>
+        <v>1000</v>
+      </c>
+      <c r="H6" s="26">
+        <f>SUM(B6:G6)</f>
+        <v>5850</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25"/>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:H1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -7845,8 +10206,8 @@
           <x14:colorLow theme="4"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Reporte Mensual Primer Año'!B5:G5</xm:f>
-              <xm:sqref>B22</xm:sqref>
+              <xm:f>'Reporte Mensual Segundo Año'!B5:G5</xm:f>
+              <xm:sqref>I5</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
@@ -7861,349 +10222,14 @@
           <x14:colorLow theme="4"/>
           <x14:sparklines>
             <x14:sparkline>
-              <xm:f>'Reporte Mensual Primer Año'!B4:G4</xm:f>
-              <xm:sqref>B21</xm:sqref>
+              <xm:f>'Reporte Mensual Segundo Año'!B4:G4</xm:f>
+              <xm:sqref>I4</xm:sqref>
             </x14:sparkline>
           </x14:sparklines>
         </x14:sparklineGroup>
       </x14:sparklineGroups>
     </ext>
   </extLst>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G10"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="2"/>
-      <c r="B3" s="24" t="s">
-        <v>6</v>
-      </c>
-      <c r="C3" s="25">
-        <f>SUM(C6:C9)</f>
-        <v>2800</v>
-      </c>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="25">
-        <f>SUM(G6:G10)</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-    </row>
-    <row r="5" spans="1:7" ht="21" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="D5" s="2"/>
-      <c r="E5" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="12">
-        <v>1200</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="32" t="s">
-        <v>8</v>
-      </c>
-      <c r="F6" s="20" t="s">
-        <v>19</v>
-      </c>
-      <c r="G6" s="12">
-        <v>300</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="21" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="13">
-        <v>100</v>
-      </c>
-      <c r="D7" s="2"/>
-      <c r="E7" s="32"/>
-      <c r="F7" s="21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G7" s="13">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="B8" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="C8" s="23">
-        <v>1200</v>
-      </c>
-      <c r="D8" s="2"/>
-      <c r="E8" s="32"/>
-      <c r="F8" s="20" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="12">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" s="29"/>
-      <c r="B9" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="13">
-        <v>300</v>
-      </c>
-      <c r="D9" s="2"/>
-      <c r="E9" s="29" t="s">
-        <v>9</v>
-      </c>
-      <c r="F9" s="21" t="s">
-        <v>21</v>
-      </c>
-      <c r="G9" s="13">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="D10" s="2"/>
-      <c r="E10" s="29"/>
-      <c r="F10" s="20" t="s">
-        <v>13</v>
-      </c>
-      <c r="G10" s="12">
-        <v>300</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="E9:E10"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="2"/>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-    </row>
-    <row r="3" spans="1:8" ht="21" x14ac:dyDescent="0.25">
-      <c r="B3" s="9" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" s="9" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="H3" s="9" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" s="10">
-        <f>SUM('Segundo Año'!C6:C7)</f>
-        <v>1300</v>
-      </c>
-      <c r="C4" s="10">
-        <f>SUM('Segundo Año'!C8:C9)</f>
-        <v>1500</v>
-      </c>
-      <c r="D4" s="12">
-        <v>0</v>
-      </c>
-      <c r="E4" s="12">
-        <v>0</v>
-      </c>
-      <c r="F4" s="12">
-        <v>0</v>
-      </c>
-      <c r="G4" s="12">
-        <v>0</v>
-      </c>
-      <c r="H4" s="26">
-        <f>SUM(B4:G4)</f>
-        <v>2800</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="11">
-        <f>SUM('Segundo Año'!G6:G8)</f>
-        <v>600</v>
-      </c>
-      <c r="C5" s="11">
-        <f>SUM('Segundo Año'!G9:G10)</f>
-        <v>400</v>
-      </c>
-      <c r="D5" s="13">
-        <v>0</v>
-      </c>
-      <c r="E5" s="13">
-        <v>0</v>
-      </c>
-      <c r="F5" s="13">
-        <v>0</v>
-      </c>
-      <c r="G5" s="13">
-        <v>0</v>
-      </c>
-      <c r="H5" s="26">
-        <f t="shared" ref="H5:H6" si="0">SUM(B5:G5)</f>
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="B6" s="14">
-        <f>B4-B5</f>
-        <v>700</v>
-      </c>
-      <c r="C6" s="14">
-        <f t="shared" ref="C6:G6" si="1">C4-C5</f>
-        <v>1100</v>
-      </c>
-      <c r="D6" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="E6" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="F6" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="G6" s="14">
-        <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="H6" s="26">
-        <f t="shared" si="0"/>
-        <v>1800</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25"/>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:H1"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -8218,16 +10244,16 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" ht="23" x14ac:dyDescent="0.25">
-      <c r="A1" s="33" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
+      <c r="A1" s="29" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="2"/>
@@ -8240,25 +10266,25 @@
     </row>
     <row r="3" spans="1:8" ht="37" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B3" s="1">
         <f>'Primer Año'!C3+'Segundo Año'!C3</f>
         <v>11950</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E3" s="1">
         <f>'Primer Año'!G3+'Segundo Año'!G3</f>
-        <v>4020</v>
+        <v>4120</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="H3" s="1">
         <f>B3-E3</f>
-        <v>7930</v>
+        <v>7830</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="20" thickTop="1" x14ac:dyDescent="0.25"/>

</xml_diff>